<commit_message>
added product_option_id and had temporary quick fix for library product price -1
</commit_message>
<xml_diff>
--- a/productImportExample2.xlsx
+++ b/productImportExample2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.gao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sale\Documents\ChemFarmImports\Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{574EE27B-77DE-4CBA-9B5F-EB094B936A79}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16788" windowHeight="7632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16788" windowHeight="7632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -646,11 +647,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>226</v>
+        <v>269</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>20</v>
@@ -801,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>29</v>
@@ -857,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>228</v>
+        <v>271</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>34</v>
@@ -913,7 +914,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>229</v>
+        <v>272</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>39</v>
@@ -969,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>230</v>
+        <v>273</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>43</v>
@@ -1025,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>47</v>
@@ -1081,7 +1082,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>232</v>
+        <v>275</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>51</v>
@@ -1137,7 +1138,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>233</v>
+        <v>276</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>55</v>
@@ -1193,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>234</v>
+        <v>277</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>59</v>

</xml_diff>